<commit_message>
yeah boi, update sur modele de donnees
</commit_message>
<xml_diff>
--- a/Documents/Classeur1.xlsx
+++ b/Documents/Classeur1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Python\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\Python\github\ERP-Systeme\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11595" firstSheet="3" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Responsabilitées" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="535" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="366">
   <si>
     <t>Membres D'équipe</t>
   </si>
@@ -1118,6 +1118,12 @@
   <si>
     <t>Pas Fait (en train de se faire)</t>
   </si>
+  <si>
+    <t>nomTable</t>
+  </si>
+  <si>
+    <t>action</t>
+  </si>
 </sst>
 </file>
 
@@ -1598,7 +1604,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="149">
+  <cellXfs count="151">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1868,6 +1874,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -34846,10 +34854,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L68"/>
+  <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -35505,72 +35513,105 @@
       <c r="F61" s="128"/>
     </row>
     <row r="62" spans="2:12" ht="15" customHeight="1">
-      <c r="B62" s="139" t="s">
+      <c r="B62" s="137" t="s">
         <v>342</v>
       </c>
-      <c r="C62" s="130"/>
-      <c r="D62" s="130"/>
-      <c r="E62" s="136" t="s">
+      <c r="C62" s="127"/>
+      <c r="D62" s="127"/>
+      <c r="E62" s="133" t="s">
         <v>302</v>
       </c>
-      <c r="F62" s="131"/>
+      <c r="F62" s="128"/>
+    </row>
+    <row r="63" spans="2:12" ht="15" customHeight="1">
+      <c r="B63" s="132" t="s">
+        <v>364</v>
+      </c>
+      <c r="C63" s="127"/>
+      <c r="D63" s="127"/>
+      <c r="E63" s="149" t="s">
+        <v>302</v>
+      </c>
+      <c r="F63" s="128"/>
     </row>
     <row r="64" spans="2:12" ht="15" customHeight="1">
-      <c r="B64" s="138" t="s">
-        <v>347</v>
-      </c>
-      <c r="C64" s="124"/>
-      <c r="D64" s="124"/>
-      <c r="E64" s="124"/>
-      <c r="F64" s="125"/>
+      <c r="B64" s="132" t="s">
+        <v>335</v>
+      </c>
+      <c r="C64" s="127"/>
+      <c r="D64" s="127"/>
+      <c r="E64" s="149" t="s">
+        <v>302</v>
+      </c>
+      <c r="F64" s="128"/>
       <c r="H64" s="123" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="65" spans="2:8" ht="15" customHeight="1">
-      <c r="B65" s="132" t="s">
-        <v>344</v>
-      </c>
-      <c r="C65" s="127"/>
-      <c r="D65" s="127"/>
-      <c r="E65" s="143" t="s">
-        <v>301</v>
-      </c>
-      <c r="F65" s="128"/>
+      <c r="B65" s="135" t="s">
+        <v>365</v>
+      </c>
+      <c r="C65" s="130"/>
+      <c r="D65" s="130"/>
+      <c r="E65" s="150" t="s">
+        <v>302</v>
+      </c>
+      <c r="F65" s="131"/>
       <c r="H65" s="123" t="s">
         <v>351</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="15" customHeight="1">
-      <c r="B66" s="132" t="s">
+    <row r="67" spans="2:8" ht="15" customHeight="1">
+      <c r="B67" s="138" t="s">
+        <v>347</v>
+      </c>
+      <c r="C67" s="124"/>
+      <c r="D67" s="124"/>
+      <c r="E67" s="124"/>
+      <c r="F67" s="125"/>
+    </row>
+    <row r="68" spans="2:8" ht="15" customHeight="1">
+      <c r="B68" s="132" t="s">
+        <v>344</v>
+      </c>
+      <c r="C68" s="127"/>
+      <c r="D68" s="127"/>
+      <c r="E68" s="143" t="s">
+        <v>301</v>
+      </c>
+      <c r="F68" s="128"/>
+    </row>
+    <row r="69" spans="2:8" ht="15" customHeight="1">
+      <c r="B69" s="132" t="s">
         <v>241</v>
       </c>
-      <c r="C66" s="127"/>
-      <c r="D66" s="127"/>
-      <c r="E66" s="143" t="s">
+      <c r="C69" s="127"/>
+      <c r="D69" s="127"/>
+      <c r="E69" s="143" t="s">
         <v>302</v>
       </c>
-      <c r="F66" s="128"/>
-    </row>
-    <row r="67" spans="2:8" ht="15" customHeight="1">
-      <c r="B67" s="132" t="s">
+      <c r="F69" s="128"/>
+    </row>
+    <row r="70" spans="2:8" ht="15" customHeight="1">
+      <c r="B70" s="132" t="s">
         <v>348</v>
       </c>
-      <c r="C67" s="127"/>
-      <c r="D67" s="127"/>
-      <c r="E67" s="143" t="s">
+      <c r="C70" s="127"/>
+      <c r="D70" s="127"/>
+      <c r="E70" s="143" t="s">
         <v>301</v>
       </c>
-      <c r="F67" s="128"/>
-    </row>
-    <row r="68" spans="2:8" ht="15" customHeight="1">
-      <c r="B68" s="135" t="s">
+      <c r="F70" s="128"/>
+    </row>
+    <row r="71" spans="2:8" ht="15" customHeight="1">
+      <c r="B71" s="135" t="s">
         <v>349</v>
       </c>
-      <c r="C68" s="130"/>
-      <c r="D68" s="130"/>
-      <c r="E68" s="130"/>
-      <c r="F68" s="131"/>
+      <c r="C71" s="130"/>
+      <c r="D71" s="130"/>
+      <c r="E71" s="130"/>
+      <c r="F71" s="131"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -35582,7 +35623,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
doc final et commencement cron jobs
</commit_message>
<xml_diff>
--- a/Documents/Classeur1.xlsx
+++ b/Documents/Classeur1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="368">
   <si>
     <t>Membres D'équipe</t>
   </si>
@@ -1124,6 +1124,12 @@
   <si>
     <t>action</t>
   </si>
+  <si>
+    <t>5h</t>
+  </si>
+  <si>
+    <t>actif</t>
+  </si>
 </sst>
 </file>
 
@@ -1604,7 +1610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="150">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1863,8 +1869,9 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1874,8 +1881,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11476,10 +11481,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="39.75" customHeight="1">
-      <c r="A1" s="144" t="s">
+      <c r="A1" s="145" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="146" t="s">
+      <c r="B1" s="147" t="s">
         <v>13</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -11497,8 +11502,8 @@
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:24" ht="6" customHeight="1">
-      <c r="A2" s="145"/>
-      <c r="B2" s="147"/>
+      <c r="A2" s="146"/>
+      <c r="B2" s="148"/>
       <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
@@ -26659,16 +26664,16 @@
       <c r="Z67" s="37"/>
     </row>
     <row r="68" spans="1:26">
-      <c r="A68" s="148"/>
-      <c r="B68" s="145"/>
-      <c r="C68" s="145"/>
-      <c r="D68" s="145"/>
-      <c r="E68" s="145"/>
-      <c r="F68" s="145"/>
-      <c r="G68" s="145"/>
-      <c r="H68" s="145"/>
-      <c r="I68" s="145"/>
-      <c r="J68" s="148"/>
+      <c r="A68" s="149"/>
+      <c r="B68" s="146"/>
+      <c r="C68" s="146"/>
+      <c r="D68" s="146"/>
+      <c r="E68" s="146"/>
+      <c r="F68" s="146"/>
+      <c r="G68" s="146"/>
+      <c r="H68" s="146"/>
+      <c r="I68" s="146"/>
+      <c r="J68" s="149"/>
       <c r="K68" s="31"/>
       <c r="L68" s="96"/>
       <c r="M68" s="96"/>
@@ -26702,7 +26707,7 @@
       </c>
       <c r="H69" s="58"/>
       <c r="I69" s="62"/>
-      <c r="J69" s="145"/>
+      <c r="J69" s="146"/>
       <c r="K69" s="98"/>
       <c r="L69" s="60" t="s">
         <v>140</v>
@@ -26738,7 +26743,7 @@
         <v>166</v>
       </c>
       <c r="I70" s="70"/>
-      <c r="J70" s="145"/>
+      <c r="J70" s="146"/>
       <c r="K70" s="98"/>
       <c r="L70" s="67"/>
       <c r="M70" s="67"/>
@@ -26770,7 +26775,7 @@
         <v>158</v>
       </c>
       <c r="I71" s="70"/>
-      <c r="J71" s="145"/>
+      <c r="J71" s="146"/>
       <c r="K71" s="98"/>
       <c r="L71" s="67"/>
       <c r="M71" s="67"/>
@@ -26798,7 +26803,7 @@
       <c r="G72" s="67"/>
       <c r="H72" s="67"/>
       <c r="I72" s="70"/>
-      <c r="J72" s="145"/>
+      <c r="J72" s="146"/>
       <c r="K72" s="98"/>
       <c r="L72" s="67"/>
       <c r="M72" s="67"/>
@@ -26826,7 +26831,7 @@
       <c r="G73" s="67"/>
       <c r="H73" s="67"/>
       <c r="I73" s="70"/>
-      <c r="J73" s="145"/>
+      <c r="J73" s="146"/>
       <c r="K73" s="98"/>
       <c r="L73" s="67"/>
       <c r="M73" s="67"/>
@@ -26854,7 +26859,7 @@
       <c r="G74" s="67"/>
       <c r="H74" s="67"/>
       <c r="I74" s="70"/>
-      <c r="J74" s="145"/>
+      <c r="J74" s="146"/>
       <c r="K74" s="98"/>
       <c r="L74" s="67"/>
       <c r="M74" s="67"/>
@@ -26884,7 +26889,7 @@
       <c r="G75" s="58"/>
       <c r="H75" s="58"/>
       <c r="I75" s="62"/>
-      <c r="J75" s="145"/>
+      <c r="J75" s="146"/>
       <c r="K75" s="98"/>
       <c r="L75" s="60" t="s">
         <v>187</v>
@@ -26914,7 +26919,7 @@
       <c r="G76" s="67"/>
       <c r="H76" s="67"/>
       <c r="I76" s="70"/>
-      <c r="J76" s="145"/>
+      <c r="J76" s="146"/>
       <c r="K76" s="98"/>
       <c r="L76" s="118" t="s">
         <v>223</v>
@@ -26944,7 +26949,7 @@
       <c r="G77" s="67"/>
       <c r="H77" s="67"/>
       <c r="I77" s="70"/>
-      <c r="J77" s="145"/>
+      <c r="J77" s="146"/>
       <c r="K77" s="98"/>
       <c r="L77" s="69" t="s">
         <v>224</v>
@@ -26974,7 +26979,7 @@
       <c r="G78" s="67"/>
       <c r="H78" s="67"/>
       <c r="I78" s="70"/>
-      <c r="J78" s="145"/>
+      <c r="J78" s="146"/>
       <c r="K78" s="98"/>
       <c r="L78" s="69" t="s">
         <v>225</v>
@@ -27004,7 +27009,7 @@
       <c r="G79" s="67"/>
       <c r="H79" s="67"/>
       <c r="I79" s="70"/>
-      <c r="J79" s="145"/>
+      <c r="J79" s="146"/>
       <c r="K79" s="98"/>
       <c r="L79" s="69" t="s">
         <v>226</v>
@@ -27034,7 +27039,7 @@
       <c r="G80" s="67"/>
       <c r="H80" s="67"/>
       <c r="I80" s="70"/>
-      <c r="J80" s="145"/>
+      <c r="J80" s="146"/>
       <c r="K80" s="98"/>
       <c r="L80" s="67"/>
       <c r="M80" s="67"/>
@@ -27062,7 +27067,7 @@
       <c r="G81" s="67"/>
       <c r="H81" s="67"/>
       <c r="I81" s="70"/>
-      <c r="J81" s="145"/>
+      <c r="J81" s="146"/>
       <c r="K81" s="98"/>
       <c r="L81" s="67"/>
       <c r="M81" s="67"/>
@@ -27090,7 +27095,7 @@
       <c r="G82" s="67"/>
       <c r="H82" s="67"/>
       <c r="I82" s="70"/>
-      <c r="J82" s="145"/>
+      <c r="J82" s="146"/>
       <c r="K82" s="98"/>
       <c r="L82" s="67"/>
       <c r="M82" s="67"/>
@@ -27118,7 +27123,7 @@
       <c r="G83" s="67"/>
       <c r="H83" s="67"/>
       <c r="I83" s="70"/>
-      <c r="J83" s="145"/>
+      <c r="J83" s="146"/>
       <c r="K83" s="98"/>
       <c r="L83" s="67"/>
       <c r="M83" s="67"/>
@@ -27146,7 +27151,7 @@
       <c r="G84" s="58"/>
       <c r="H84" s="58"/>
       <c r="I84" s="62"/>
-      <c r="J84" s="145"/>
+      <c r="J84" s="146"/>
       <c r="K84" s="98"/>
       <c r="L84" s="67"/>
       <c r="M84" s="67"/>
@@ -27176,7 +27181,7 @@
       </c>
       <c r="H85" s="67"/>
       <c r="I85" s="78"/>
-      <c r="J85" s="145"/>
+      <c r="J85" s="146"/>
       <c r="K85" s="98"/>
       <c r="L85" s="67"/>
       <c r="M85" s="67"/>
@@ -27206,7 +27211,7 @@
       <c r="G86" s="67"/>
       <c r="H86" s="67"/>
       <c r="I86" s="70"/>
-      <c r="J86" s="145"/>
+      <c r="J86" s="146"/>
       <c r="K86" s="98"/>
       <c r="L86" s="67"/>
       <c r="M86" s="67"/>
@@ -27234,7 +27239,7 @@
       <c r="G87" s="58"/>
       <c r="H87" s="58"/>
       <c r="I87" s="62"/>
-      <c r="J87" s="145"/>
+      <c r="J87" s="146"/>
       <c r="K87" s="98"/>
       <c r="L87" s="58"/>
       <c r="M87" s="58"/>
@@ -27253,16 +27258,16 @@
       <c r="Z87" s="37"/>
     </row>
     <row r="88" spans="1:26">
-      <c r="A88" s="148"/>
-      <c r="B88" s="145"/>
-      <c r="C88" s="145"/>
-      <c r="D88" s="145"/>
-      <c r="E88" s="145"/>
-      <c r="F88" s="145"/>
-      <c r="G88" s="145"/>
-      <c r="H88" s="145"/>
-      <c r="I88" s="145"/>
-      <c r="J88" s="145"/>
+      <c r="A88" s="149"/>
+      <c r="B88" s="146"/>
+      <c r="C88" s="146"/>
+      <c r="D88" s="146"/>
+      <c r="E88" s="146"/>
+      <c r="F88" s="146"/>
+      <c r="G88" s="146"/>
+      <c r="H88" s="146"/>
+      <c r="I88" s="146"/>
+      <c r="J88" s="146"/>
       <c r="K88" s="31"/>
       <c r="L88" s="96"/>
       <c r="M88" s="96"/>
@@ -27281,16 +27286,16 @@
       <c r="Z88" s="37"/>
     </row>
     <row r="89" spans="1:26" ht="26.25">
-      <c r="A89" s="145"/>
-      <c r="B89" s="145"/>
-      <c r="C89" s="145"/>
-      <c r="D89" s="145"/>
-      <c r="E89" s="145"/>
-      <c r="F89" s="145"/>
-      <c r="G89" s="145"/>
-      <c r="H89" s="145"/>
-      <c r="I89" s="145"/>
-      <c r="J89" s="145"/>
+      <c r="A89" s="146"/>
+      <c r="B89" s="146"/>
+      <c r="C89" s="146"/>
+      <c r="D89" s="146"/>
+      <c r="E89" s="146"/>
+      <c r="F89" s="146"/>
+      <c r="G89" s="146"/>
+      <c r="H89" s="146"/>
+      <c r="I89" s="146"/>
+      <c r="J89" s="146"/>
       <c r="K89" s="98"/>
       <c r="L89" s="60" t="s">
         <v>140</v>
@@ -27315,16 +27320,16 @@
       <c r="Z89" s="37"/>
     </row>
     <row r="90" spans="1:26">
-      <c r="A90" s="145"/>
-      <c r="B90" s="145"/>
-      <c r="C90" s="145"/>
-      <c r="D90" s="145"/>
-      <c r="E90" s="145"/>
-      <c r="F90" s="145"/>
-      <c r="G90" s="145"/>
-      <c r="H90" s="145"/>
-      <c r="I90" s="145"/>
-      <c r="J90" s="145"/>
+      <c r="A90" s="146"/>
+      <c r="B90" s="146"/>
+      <c r="C90" s="146"/>
+      <c r="D90" s="146"/>
+      <c r="E90" s="146"/>
+      <c r="F90" s="146"/>
+      <c r="G90" s="146"/>
+      <c r="H90" s="146"/>
+      <c r="I90" s="146"/>
+      <c r="J90" s="146"/>
       <c r="K90" s="98"/>
       <c r="L90" s="67"/>
       <c r="M90" s="67"/>
@@ -27345,16 +27350,16 @@
       <c r="Z90" s="37"/>
     </row>
     <row r="91" spans="1:26">
-      <c r="A91" s="145"/>
-      <c r="B91" s="145"/>
-      <c r="C91" s="145"/>
-      <c r="D91" s="145"/>
-      <c r="E91" s="145"/>
-      <c r="F91" s="145"/>
-      <c r="G91" s="145"/>
-      <c r="H91" s="145"/>
-      <c r="I91" s="145"/>
-      <c r="J91" s="145"/>
+      <c r="A91" s="146"/>
+      <c r="B91" s="146"/>
+      <c r="C91" s="146"/>
+      <c r="D91" s="146"/>
+      <c r="E91" s="146"/>
+      <c r="F91" s="146"/>
+      <c r="G91" s="146"/>
+      <c r="H91" s="146"/>
+      <c r="I91" s="146"/>
+      <c r="J91" s="146"/>
       <c r="K91" s="98"/>
       <c r="L91" s="67"/>
       <c r="M91" s="67"/>
@@ -27373,16 +27378,16 @@
       <c r="Z91" s="37"/>
     </row>
     <row r="92" spans="1:26">
-      <c r="A92" s="145"/>
-      <c r="B92" s="145"/>
-      <c r="C92" s="145"/>
-      <c r="D92" s="145"/>
-      <c r="E92" s="145"/>
-      <c r="F92" s="145"/>
-      <c r="G92" s="145"/>
-      <c r="H92" s="145"/>
-      <c r="I92" s="145"/>
-      <c r="J92" s="145"/>
+      <c r="A92" s="146"/>
+      <c r="B92" s="146"/>
+      <c r="C92" s="146"/>
+      <c r="D92" s="146"/>
+      <c r="E92" s="146"/>
+      <c r="F92" s="146"/>
+      <c r="G92" s="146"/>
+      <c r="H92" s="146"/>
+      <c r="I92" s="146"/>
+      <c r="J92" s="146"/>
       <c r="K92" s="98"/>
       <c r="L92" s="67"/>
       <c r="M92" s="67"/>
@@ -27401,16 +27406,16 @@
       <c r="Z92" s="37"/>
     </row>
     <row r="93" spans="1:26">
-      <c r="A93" s="145"/>
-      <c r="B93" s="145"/>
-      <c r="C93" s="145"/>
-      <c r="D93" s="145"/>
-      <c r="E93" s="145"/>
-      <c r="F93" s="145"/>
-      <c r="G93" s="145"/>
-      <c r="H93" s="145"/>
-      <c r="I93" s="145"/>
-      <c r="J93" s="145"/>
+      <c r="A93" s="146"/>
+      <c r="B93" s="146"/>
+      <c r="C93" s="146"/>
+      <c r="D93" s="146"/>
+      <c r="E93" s="146"/>
+      <c r="F93" s="146"/>
+      <c r="G93" s="146"/>
+      <c r="H93" s="146"/>
+      <c r="I93" s="146"/>
+      <c r="J93" s="146"/>
       <c r="K93" s="98"/>
       <c r="L93" s="67"/>
       <c r="M93" s="67"/>
@@ -27429,16 +27434,16 @@
       <c r="Z93" s="37"/>
     </row>
     <row r="94" spans="1:26">
-      <c r="A94" s="145"/>
-      <c r="B94" s="145"/>
-      <c r="C94" s="145"/>
-      <c r="D94" s="145"/>
-      <c r="E94" s="145"/>
-      <c r="F94" s="145"/>
-      <c r="G94" s="145"/>
-      <c r="H94" s="145"/>
-      <c r="I94" s="145"/>
-      <c r="J94" s="145"/>
+      <c r="A94" s="146"/>
+      <c r="B94" s="146"/>
+      <c r="C94" s="146"/>
+      <c r="D94" s="146"/>
+      <c r="E94" s="146"/>
+      <c r="F94" s="146"/>
+      <c r="G94" s="146"/>
+      <c r="H94" s="146"/>
+      <c r="I94" s="146"/>
+      <c r="J94" s="146"/>
       <c r="K94" s="98"/>
       <c r="L94" s="67"/>
       <c r="M94" s="67"/>
@@ -27457,16 +27462,16 @@
       <c r="Z94" s="37"/>
     </row>
     <row r="95" spans="1:26">
-      <c r="A95" s="145"/>
-      <c r="B95" s="145"/>
-      <c r="C95" s="145"/>
-      <c r="D95" s="145"/>
-      <c r="E95" s="145"/>
-      <c r="F95" s="145"/>
-      <c r="G95" s="145"/>
-      <c r="H95" s="145"/>
-      <c r="I95" s="145"/>
-      <c r="J95" s="145"/>
+      <c r="A95" s="146"/>
+      <c r="B95" s="146"/>
+      <c r="C95" s="146"/>
+      <c r="D95" s="146"/>
+      <c r="E95" s="146"/>
+      <c r="F95" s="146"/>
+      <c r="G95" s="146"/>
+      <c r="H95" s="146"/>
+      <c r="I95" s="146"/>
+      <c r="J95" s="146"/>
       <c r="K95" s="98"/>
       <c r="L95" s="60" t="s">
         <v>187</v>
@@ -27489,16 +27494,16 @@
       <c r="Z95" s="37"/>
     </row>
     <row r="96" spans="1:26">
-      <c r="A96" s="145"/>
-      <c r="B96" s="145"/>
-      <c r="C96" s="145"/>
-      <c r="D96" s="145"/>
-      <c r="E96" s="145"/>
-      <c r="F96" s="145"/>
-      <c r="G96" s="145"/>
-      <c r="H96" s="145"/>
-      <c r="I96" s="145"/>
-      <c r="J96" s="145"/>
+      <c r="A96" s="146"/>
+      <c r="B96" s="146"/>
+      <c r="C96" s="146"/>
+      <c r="D96" s="146"/>
+      <c r="E96" s="146"/>
+      <c r="F96" s="146"/>
+      <c r="G96" s="146"/>
+      <c r="H96" s="146"/>
+      <c r="I96" s="146"/>
+      <c r="J96" s="146"/>
       <c r="K96" s="98"/>
       <c r="L96" s="69" t="s">
         <v>235</v>
@@ -27519,16 +27524,16 @@
       <c r="Z96" s="37"/>
     </row>
     <row r="97" spans="1:26">
-      <c r="A97" s="145"/>
-      <c r="B97" s="145"/>
-      <c r="C97" s="145"/>
-      <c r="D97" s="145"/>
-      <c r="E97" s="145"/>
-      <c r="F97" s="145"/>
-      <c r="G97" s="145"/>
-      <c r="H97" s="145"/>
-      <c r="I97" s="145"/>
-      <c r="J97" s="145"/>
+      <c r="A97" s="146"/>
+      <c r="B97" s="146"/>
+      <c r="C97" s="146"/>
+      <c r="D97" s="146"/>
+      <c r="E97" s="146"/>
+      <c r="F97" s="146"/>
+      <c r="G97" s="146"/>
+      <c r="H97" s="146"/>
+      <c r="I97" s="146"/>
+      <c r="J97" s="146"/>
       <c r="K97" s="98"/>
       <c r="L97" s="69" t="s">
         <v>236</v>
@@ -27551,16 +27556,16 @@
       <c r="Z97" s="37"/>
     </row>
     <row r="98" spans="1:26">
-      <c r="A98" s="145"/>
-      <c r="B98" s="145"/>
-      <c r="C98" s="145"/>
-      <c r="D98" s="145"/>
-      <c r="E98" s="145"/>
-      <c r="F98" s="145"/>
-      <c r="G98" s="145"/>
-      <c r="H98" s="145"/>
-      <c r="I98" s="145"/>
-      <c r="J98" s="145"/>
+      <c r="A98" s="146"/>
+      <c r="B98" s="146"/>
+      <c r="C98" s="146"/>
+      <c r="D98" s="146"/>
+      <c r="E98" s="146"/>
+      <c r="F98" s="146"/>
+      <c r="G98" s="146"/>
+      <c r="H98" s="146"/>
+      <c r="I98" s="146"/>
+      <c r="J98" s="146"/>
       <c r="K98" s="98"/>
       <c r="L98" s="67"/>
       <c r="M98" s="67"/>
@@ -27579,16 +27584,16 @@
       <c r="Z98" s="37"/>
     </row>
     <row r="99" spans="1:26">
-      <c r="A99" s="145"/>
-      <c r="B99" s="145"/>
-      <c r="C99" s="145"/>
-      <c r="D99" s="145"/>
-      <c r="E99" s="145"/>
-      <c r="F99" s="145"/>
-      <c r="G99" s="145"/>
-      <c r="H99" s="145"/>
-      <c r="I99" s="145"/>
-      <c r="J99" s="145"/>
+      <c r="A99" s="146"/>
+      <c r="B99" s="146"/>
+      <c r="C99" s="146"/>
+      <c r="D99" s="146"/>
+      <c r="E99" s="146"/>
+      <c r="F99" s="146"/>
+      <c r="G99" s="146"/>
+      <c r="H99" s="146"/>
+      <c r="I99" s="146"/>
+      <c r="J99" s="146"/>
       <c r="K99" s="98"/>
       <c r="L99" s="69" t="s">
         <v>239</v>
@@ -27609,16 +27614,16 @@
       <c r="Z99" s="37"/>
     </row>
     <row r="100" spans="1:26">
-      <c r="A100" s="145"/>
-      <c r="B100" s="145"/>
-      <c r="C100" s="145"/>
-      <c r="D100" s="145"/>
-      <c r="E100" s="145"/>
-      <c r="F100" s="145"/>
-      <c r="G100" s="145"/>
-      <c r="H100" s="145"/>
-      <c r="I100" s="145"/>
-      <c r="J100" s="145"/>
+      <c r="A100" s="146"/>
+      <c r="B100" s="146"/>
+      <c r="C100" s="146"/>
+      <c r="D100" s="146"/>
+      <c r="E100" s="146"/>
+      <c r="F100" s="146"/>
+      <c r="G100" s="146"/>
+      <c r="H100" s="146"/>
+      <c r="I100" s="146"/>
+      <c r="J100" s="146"/>
       <c r="K100" s="98"/>
       <c r="L100" s="69" t="s">
         <v>240</v>
@@ -27641,16 +27646,16 @@
       <c r="Z100" s="37"/>
     </row>
     <row r="101" spans="1:26">
-      <c r="A101" s="145"/>
-      <c r="B101" s="145"/>
-      <c r="C101" s="145"/>
-      <c r="D101" s="145"/>
-      <c r="E101" s="145"/>
-      <c r="F101" s="145"/>
-      <c r="G101" s="145"/>
-      <c r="H101" s="145"/>
-      <c r="I101" s="145"/>
-      <c r="J101" s="145"/>
+      <c r="A101" s="146"/>
+      <c r="B101" s="146"/>
+      <c r="C101" s="146"/>
+      <c r="D101" s="146"/>
+      <c r="E101" s="146"/>
+      <c r="F101" s="146"/>
+      <c r="G101" s="146"/>
+      <c r="H101" s="146"/>
+      <c r="I101" s="146"/>
+      <c r="J101" s="146"/>
       <c r="K101" s="98"/>
       <c r="L101" s="69" t="s">
         <v>242</v>
@@ -27673,16 +27678,16 @@
       <c r="Z101" s="37"/>
     </row>
     <row r="102" spans="1:26">
-      <c r="A102" s="145"/>
-      <c r="B102" s="145"/>
-      <c r="C102" s="145"/>
-      <c r="D102" s="145"/>
-      <c r="E102" s="145"/>
-      <c r="F102" s="145"/>
-      <c r="G102" s="145"/>
-      <c r="H102" s="145"/>
-      <c r="I102" s="145"/>
-      <c r="J102" s="145"/>
+      <c r="A102" s="146"/>
+      <c r="B102" s="146"/>
+      <c r="C102" s="146"/>
+      <c r="D102" s="146"/>
+      <c r="E102" s="146"/>
+      <c r="F102" s="146"/>
+      <c r="G102" s="146"/>
+      <c r="H102" s="146"/>
+      <c r="I102" s="146"/>
+      <c r="J102" s="146"/>
       <c r="K102" s="98"/>
       <c r="L102" s="69" t="s">
         <v>243</v>
@@ -27703,16 +27708,16 @@
       <c r="Z102" s="37"/>
     </row>
     <row r="103" spans="1:26">
-      <c r="A103" s="145"/>
-      <c r="B103" s="145"/>
-      <c r="C103" s="145"/>
-      <c r="D103" s="145"/>
-      <c r="E103" s="145"/>
-      <c r="F103" s="145"/>
-      <c r="G103" s="145"/>
-      <c r="H103" s="145"/>
-      <c r="I103" s="145"/>
-      <c r="J103" s="145"/>
+      <c r="A103" s="146"/>
+      <c r="B103" s="146"/>
+      <c r="C103" s="146"/>
+      <c r="D103" s="146"/>
+      <c r="E103" s="146"/>
+      <c r="F103" s="146"/>
+      <c r="G103" s="146"/>
+      <c r="H103" s="146"/>
+      <c r="I103" s="146"/>
+      <c r="J103" s="146"/>
       <c r="K103" s="98"/>
       <c r="L103" s="69" t="s">
         <v>244</v>
@@ -27733,16 +27738,16 @@
       <c r="Z103" s="37"/>
     </row>
     <row r="104" spans="1:26">
-      <c r="A104" s="145"/>
-      <c r="B104" s="145"/>
-      <c r="C104" s="145"/>
-      <c r="D104" s="145"/>
-      <c r="E104" s="145"/>
-      <c r="F104" s="145"/>
-      <c r="G104" s="145"/>
-      <c r="H104" s="145"/>
-      <c r="I104" s="145"/>
-      <c r="J104" s="145"/>
+      <c r="A104" s="146"/>
+      <c r="B104" s="146"/>
+      <c r="C104" s="146"/>
+      <c r="D104" s="146"/>
+      <c r="E104" s="146"/>
+      <c r="F104" s="146"/>
+      <c r="G104" s="146"/>
+      <c r="H104" s="146"/>
+      <c r="I104" s="146"/>
+      <c r="J104" s="146"/>
       <c r="K104" s="98"/>
       <c r="L104" s="69" t="s">
         <v>245</v>
@@ -27763,16 +27768,16 @@
       <c r="Z104" s="37"/>
     </row>
     <row r="105" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A105" s="145"/>
-      <c r="B105" s="145"/>
-      <c r="C105" s="145"/>
-      <c r="D105" s="145"/>
-      <c r="E105" s="145"/>
-      <c r="F105" s="145"/>
-      <c r="G105" s="145"/>
-      <c r="H105" s="145"/>
-      <c r="I105" s="145"/>
-      <c r="J105" s="145"/>
+      <c r="A105" s="146"/>
+      <c r="B105" s="146"/>
+      <c r="C105" s="146"/>
+      <c r="D105" s="146"/>
+      <c r="E105" s="146"/>
+      <c r="F105" s="146"/>
+      <c r="G105" s="146"/>
+      <c r="H105" s="146"/>
+      <c r="I105" s="146"/>
+      <c r="J105" s="146"/>
       <c r="K105" s="98"/>
       <c r="L105" s="67"/>
       <c r="M105" s="67"/>
@@ -27791,16 +27796,16 @@
       <c r="Z105" s="37"/>
     </row>
     <row r="106" spans="1:26">
-      <c r="A106" s="145"/>
-      <c r="B106" s="145"/>
-      <c r="C106" s="145"/>
-      <c r="D106" s="145"/>
-      <c r="E106" s="145"/>
-      <c r="F106" s="145"/>
-      <c r="G106" s="145"/>
-      <c r="H106" s="145"/>
-      <c r="I106" s="145"/>
-      <c r="J106" s="145"/>
+      <c r="A106" s="146"/>
+      <c r="B106" s="146"/>
+      <c r="C106" s="146"/>
+      <c r="D106" s="146"/>
+      <c r="E106" s="146"/>
+      <c r="F106" s="146"/>
+      <c r="G106" s="146"/>
+      <c r="H106" s="146"/>
+      <c r="I106" s="146"/>
+      <c r="J106" s="146"/>
       <c r="K106" s="98"/>
       <c r="L106" s="67"/>
       <c r="M106" s="67"/>
@@ -27819,16 +27824,16 @@
       <c r="Z106" s="37"/>
     </row>
     <row r="107" spans="1:26">
-      <c r="A107" s="145"/>
-      <c r="B107" s="145"/>
-      <c r="C107" s="145"/>
-      <c r="D107" s="145"/>
-      <c r="E107" s="145"/>
-      <c r="F107" s="145"/>
-      <c r="G107" s="145"/>
-      <c r="H107" s="145"/>
-      <c r="I107" s="145"/>
-      <c r="J107" s="145"/>
+      <c r="A107" s="146"/>
+      <c r="B107" s="146"/>
+      <c r="C107" s="146"/>
+      <c r="D107" s="146"/>
+      <c r="E107" s="146"/>
+      <c r="F107" s="146"/>
+      <c r="G107" s="146"/>
+      <c r="H107" s="146"/>
+      <c r="I107" s="146"/>
+      <c r="J107" s="146"/>
       <c r="K107" s="98"/>
       <c r="L107" s="67"/>
       <c r="M107" s="67"/>
@@ -27847,16 +27852,16 @@
       <c r="Z107" s="37"/>
     </row>
     <row r="108" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A108" s="145"/>
-      <c r="B108" s="145"/>
-      <c r="C108" s="145"/>
-      <c r="D108" s="145"/>
-      <c r="E108" s="145"/>
-      <c r="F108" s="145"/>
-      <c r="G108" s="145"/>
-      <c r="H108" s="145"/>
-      <c r="I108" s="145"/>
-      <c r="J108" s="145"/>
+      <c r="A108" s="146"/>
+      <c r="B108" s="146"/>
+      <c r="C108" s="146"/>
+      <c r="D108" s="146"/>
+      <c r="E108" s="146"/>
+      <c r="F108" s="146"/>
+      <c r="G108" s="146"/>
+      <c r="H108" s="146"/>
+      <c r="I108" s="146"/>
+      <c r="J108" s="146"/>
       <c r="K108" s="98"/>
       <c r="L108" s="67"/>
       <c r="M108" s="67"/>
@@ -27877,16 +27882,16 @@
       <c r="Z108" s="37"/>
     </row>
     <row r="109" spans="1:26" ht="30.75" customHeight="1">
-      <c r="A109" s="145"/>
-      <c r="B109" s="145"/>
-      <c r="C109" s="145"/>
-      <c r="D109" s="145"/>
-      <c r="E109" s="145"/>
-      <c r="F109" s="145"/>
-      <c r="G109" s="145"/>
-      <c r="H109" s="145"/>
-      <c r="I109" s="145"/>
-      <c r="J109" s="145"/>
+      <c r="A109" s="146"/>
+      <c r="B109" s="146"/>
+      <c r="C109" s="146"/>
+      <c r="D109" s="146"/>
+      <c r="E109" s="146"/>
+      <c r="F109" s="146"/>
+      <c r="G109" s="146"/>
+      <c r="H109" s="146"/>
+      <c r="I109" s="146"/>
+      <c r="J109" s="146"/>
       <c r="K109" s="98"/>
       <c r="L109" s="67"/>
       <c r="M109" s="67"/>
@@ -27905,16 +27910,16 @@
       <c r="Z109" s="37"/>
     </row>
     <row r="110" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A110" s="145"/>
-      <c r="B110" s="145"/>
-      <c r="C110" s="145"/>
-      <c r="D110" s="145"/>
-      <c r="E110" s="145"/>
-      <c r="F110" s="145"/>
-      <c r="G110" s="145"/>
-      <c r="H110" s="145"/>
-      <c r="I110" s="145"/>
-      <c r="J110" s="145"/>
+      <c r="A110" s="146"/>
+      <c r="B110" s="146"/>
+      <c r="C110" s="146"/>
+      <c r="D110" s="146"/>
+      <c r="E110" s="146"/>
+      <c r="F110" s="146"/>
+      <c r="G110" s="146"/>
+      <c r="H110" s="146"/>
+      <c r="I110" s="146"/>
+      <c r="J110" s="146"/>
       <c r="K110" s="98"/>
       <c r="L110" s="58"/>
       <c r="M110" s="58"/>
@@ -27933,16 +27938,16 @@
       <c r="Z110" s="37"/>
     </row>
     <row r="111" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A111" s="145"/>
-      <c r="B111" s="145"/>
-      <c r="C111" s="145"/>
-      <c r="D111" s="145"/>
-      <c r="E111" s="145"/>
-      <c r="F111" s="145"/>
-      <c r="G111" s="145"/>
-      <c r="H111" s="145"/>
-      <c r="I111" s="145"/>
-      <c r="J111" s="145"/>
+      <c r="A111" s="146"/>
+      <c r="B111" s="146"/>
+      <c r="C111" s="146"/>
+      <c r="D111" s="146"/>
+      <c r="E111" s="146"/>
+      <c r="F111" s="146"/>
+      <c r="G111" s="146"/>
+      <c r="H111" s="146"/>
+      <c r="I111" s="146"/>
+      <c r="J111" s="146"/>
       <c r="K111" s="31"/>
       <c r="L111" s="31"/>
       <c r="M111" s="31"/>
@@ -27961,16 +27966,16 @@
       <c r="Z111" s="37"/>
     </row>
     <row r="112" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A112" s="145"/>
-      <c r="B112" s="145"/>
-      <c r="C112" s="145"/>
-      <c r="D112" s="145"/>
-      <c r="E112" s="145"/>
-      <c r="F112" s="145"/>
-      <c r="G112" s="145"/>
-      <c r="H112" s="145"/>
-      <c r="I112" s="145"/>
-      <c r="J112" s="145"/>
+      <c r="A112" s="146"/>
+      <c r="B112" s="146"/>
+      <c r="C112" s="146"/>
+      <c r="D112" s="146"/>
+      <c r="E112" s="146"/>
+      <c r="F112" s="146"/>
+      <c r="G112" s="146"/>
+      <c r="H112" s="146"/>
+      <c r="I112" s="146"/>
+      <c r="J112" s="146"/>
       <c r="K112" s="31"/>
       <c r="L112" s="31"/>
       <c r="M112" s="31"/>
@@ -27989,16 +27994,16 @@
       <c r="Z112" s="37"/>
     </row>
     <row r="113" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A113" s="145"/>
-      <c r="B113" s="145"/>
-      <c r="C113" s="145"/>
-      <c r="D113" s="145"/>
-      <c r="E113" s="145"/>
-      <c r="F113" s="145"/>
-      <c r="G113" s="145"/>
-      <c r="H113" s="145"/>
-      <c r="I113" s="145"/>
-      <c r="J113" s="145"/>
+      <c r="A113" s="146"/>
+      <c r="B113" s="146"/>
+      <c r="C113" s="146"/>
+      <c r="D113" s="146"/>
+      <c r="E113" s="146"/>
+      <c r="F113" s="146"/>
+      <c r="G113" s="146"/>
+      <c r="H113" s="146"/>
+      <c r="I113" s="146"/>
+      <c r="J113" s="146"/>
       <c r="K113" s="31"/>
       <c r="L113" s="31"/>
       <c r="M113" s="31"/>
@@ -28017,16 +28022,16 @@
       <c r="Z113" s="37"/>
     </row>
     <row r="114" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A114" s="145"/>
-      <c r="B114" s="145"/>
-      <c r="C114" s="145"/>
-      <c r="D114" s="145"/>
-      <c r="E114" s="145"/>
-      <c r="F114" s="145"/>
-      <c r="G114" s="145"/>
-      <c r="H114" s="145"/>
-      <c r="I114" s="145"/>
-      <c r="J114" s="145"/>
+      <c r="A114" s="146"/>
+      <c r="B114" s="146"/>
+      <c r="C114" s="146"/>
+      <c r="D114" s="146"/>
+      <c r="E114" s="146"/>
+      <c r="F114" s="146"/>
+      <c r="G114" s="146"/>
+      <c r="H114" s="146"/>
+      <c r="I114" s="146"/>
+      <c r="J114" s="146"/>
       <c r="K114" s="37"/>
       <c r="L114" s="60" t="s">
         <v>140</v>
@@ -28051,16 +28056,16 @@
       <c r="Z114" s="37"/>
     </row>
     <row r="115" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A115" s="145"/>
-      <c r="B115" s="145"/>
-      <c r="C115" s="145"/>
-      <c r="D115" s="145"/>
-      <c r="E115" s="145"/>
-      <c r="F115" s="145"/>
-      <c r="G115" s="145"/>
-      <c r="H115" s="145"/>
-      <c r="I115" s="145"/>
-      <c r="J115" s="145"/>
+      <c r="A115" s="146"/>
+      <c r="B115" s="146"/>
+      <c r="C115" s="146"/>
+      <c r="D115" s="146"/>
+      <c r="E115" s="146"/>
+      <c r="F115" s="146"/>
+      <c r="G115" s="146"/>
+      <c r="H115" s="146"/>
+      <c r="I115" s="146"/>
+      <c r="J115" s="146"/>
       <c r="K115" s="37"/>
       <c r="L115" s="67"/>
       <c r="M115" s="67"/>
@@ -28081,16 +28086,16 @@
       <c r="Z115" s="37"/>
     </row>
     <row r="116" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A116" s="145"/>
-      <c r="B116" s="145"/>
-      <c r="C116" s="145"/>
-      <c r="D116" s="145"/>
-      <c r="E116" s="145"/>
-      <c r="F116" s="145"/>
-      <c r="G116" s="145"/>
-      <c r="H116" s="145"/>
-      <c r="I116" s="145"/>
-      <c r="J116" s="145"/>
+      <c r="A116" s="146"/>
+      <c r="B116" s="146"/>
+      <c r="C116" s="146"/>
+      <c r="D116" s="146"/>
+      <c r="E116" s="146"/>
+      <c r="F116" s="146"/>
+      <c r="G116" s="146"/>
+      <c r="H116" s="146"/>
+      <c r="I116" s="146"/>
+      <c r="J116" s="146"/>
       <c r="K116" s="37"/>
       <c r="L116" s="67"/>
       <c r="M116" s="67"/>
@@ -28109,16 +28114,16 @@
       <c r="Z116" s="37"/>
     </row>
     <row r="117" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A117" s="145"/>
-      <c r="B117" s="145"/>
-      <c r="C117" s="145"/>
-      <c r="D117" s="145"/>
-      <c r="E117" s="145"/>
-      <c r="F117" s="145"/>
-      <c r="G117" s="145"/>
-      <c r="H117" s="145"/>
-      <c r="I117" s="145"/>
-      <c r="J117" s="145"/>
+      <c r="A117" s="146"/>
+      <c r="B117" s="146"/>
+      <c r="C117" s="146"/>
+      <c r="D117" s="146"/>
+      <c r="E117" s="146"/>
+      <c r="F117" s="146"/>
+      <c r="G117" s="146"/>
+      <c r="H117" s="146"/>
+      <c r="I117" s="146"/>
+      <c r="J117" s="146"/>
       <c r="K117" s="37"/>
       <c r="L117" s="67"/>
       <c r="M117" s="67"/>
@@ -28137,16 +28142,16 @@
       <c r="Z117" s="37"/>
     </row>
     <row r="118" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A118" s="145"/>
-      <c r="B118" s="145"/>
-      <c r="C118" s="145"/>
-      <c r="D118" s="145"/>
-      <c r="E118" s="145"/>
-      <c r="F118" s="145"/>
-      <c r="G118" s="145"/>
-      <c r="H118" s="145"/>
-      <c r="I118" s="145"/>
-      <c r="J118" s="145"/>
+      <c r="A118" s="146"/>
+      <c r="B118" s="146"/>
+      <c r="C118" s="146"/>
+      <c r="D118" s="146"/>
+      <c r="E118" s="146"/>
+      <c r="F118" s="146"/>
+      <c r="G118" s="146"/>
+      <c r="H118" s="146"/>
+      <c r="I118" s="146"/>
+      <c r="J118" s="146"/>
       <c r="K118" s="37"/>
       <c r="L118" s="67"/>
       <c r="M118" s="67"/>
@@ -28165,16 +28170,16 @@
       <c r="Z118" s="37"/>
     </row>
     <row r="119" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A119" s="145"/>
-      <c r="B119" s="145"/>
-      <c r="C119" s="145"/>
-      <c r="D119" s="145"/>
-      <c r="E119" s="145"/>
-      <c r="F119" s="145"/>
-      <c r="G119" s="145"/>
-      <c r="H119" s="145"/>
-      <c r="I119" s="145"/>
-      <c r="J119" s="145"/>
+      <c r="A119" s="146"/>
+      <c r="B119" s="146"/>
+      <c r="C119" s="146"/>
+      <c r="D119" s="146"/>
+      <c r="E119" s="146"/>
+      <c r="F119" s="146"/>
+      <c r="G119" s="146"/>
+      <c r="H119" s="146"/>
+      <c r="I119" s="146"/>
+      <c r="J119" s="146"/>
       <c r="K119" s="37"/>
       <c r="L119" s="67"/>
       <c r="M119" s="67"/>
@@ -28193,16 +28198,16 @@
       <c r="Z119" s="37"/>
     </row>
     <row r="120" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A120" s="145"/>
-      <c r="B120" s="145"/>
-      <c r="C120" s="145"/>
-      <c r="D120" s="145"/>
-      <c r="E120" s="145"/>
-      <c r="F120" s="145"/>
-      <c r="G120" s="145"/>
-      <c r="H120" s="145"/>
-      <c r="I120" s="145"/>
-      <c r="J120" s="145"/>
+      <c r="A120" s="146"/>
+      <c r="B120" s="146"/>
+      <c r="C120" s="146"/>
+      <c r="D120" s="146"/>
+      <c r="E120" s="146"/>
+      <c r="F120" s="146"/>
+      <c r="G120" s="146"/>
+      <c r="H120" s="146"/>
+      <c r="I120" s="146"/>
+      <c r="J120" s="146"/>
       <c r="K120" s="37"/>
       <c r="L120" s="60" t="s">
         <v>187</v>
@@ -28225,16 +28230,16 @@
       <c r="Z120" s="37"/>
     </row>
     <row r="121" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A121" s="145"/>
-      <c r="B121" s="145"/>
-      <c r="C121" s="145"/>
-      <c r="D121" s="145"/>
-      <c r="E121" s="145"/>
-      <c r="F121" s="145"/>
-      <c r="G121" s="145"/>
-      <c r="H121" s="145"/>
-      <c r="I121" s="145"/>
-      <c r="J121" s="145"/>
+      <c r="A121" s="146"/>
+      <c r="B121" s="146"/>
+      <c r="C121" s="146"/>
+      <c r="D121" s="146"/>
+      <c r="E121" s="146"/>
+      <c r="F121" s="146"/>
+      <c r="G121" s="146"/>
+      <c r="H121" s="146"/>
+      <c r="I121" s="146"/>
+      <c r="J121" s="146"/>
       <c r="K121" s="37"/>
       <c r="L121" s="118" t="s">
         <v>280</v>
@@ -28257,16 +28262,16 @@
       <c r="Z121" s="37"/>
     </row>
     <row r="122" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A122" s="145"/>
-      <c r="B122" s="145"/>
-      <c r="C122" s="145"/>
-      <c r="D122" s="145"/>
-      <c r="E122" s="145"/>
-      <c r="F122" s="145"/>
-      <c r="G122" s="145"/>
-      <c r="H122" s="145"/>
-      <c r="I122" s="145"/>
-      <c r="J122" s="145"/>
+      <c r="A122" s="146"/>
+      <c r="B122" s="146"/>
+      <c r="C122" s="146"/>
+      <c r="D122" s="146"/>
+      <c r="E122" s="146"/>
+      <c r="F122" s="146"/>
+      <c r="G122" s="146"/>
+      <c r="H122" s="146"/>
+      <c r="I122" s="146"/>
+      <c r="J122" s="146"/>
       <c r="K122" s="37"/>
       <c r="L122" s="69" t="s">
         <v>208</v>
@@ -28289,16 +28294,16 @@
       <c r="Z122" s="37"/>
     </row>
     <row r="123" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A123" s="145"/>
-      <c r="B123" s="145"/>
-      <c r="C123" s="145"/>
-      <c r="D123" s="145"/>
-      <c r="E123" s="145"/>
-      <c r="F123" s="145"/>
-      <c r="G123" s="145"/>
-      <c r="H123" s="145"/>
-      <c r="I123" s="145"/>
-      <c r="J123" s="145"/>
+      <c r="A123" s="146"/>
+      <c r="B123" s="146"/>
+      <c r="C123" s="146"/>
+      <c r="D123" s="146"/>
+      <c r="E123" s="146"/>
+      <c r="F123" s="146"/>
+      <c r="G123" s="146"/>
+      <c r="H123" s="146"/>
+      <c r="I123" s="146"/>
+      <c r="J123" s="146"/>
       <c r="K123" s="37"/>
       <c r="L123" s="69" t="s">
         <v>210</v>
@@ -28321,16 +28326,16 @@
       <c r="Z123" s="37"/>
     </row>
     <row r="124" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A124" s="145"/>
-      <c r="B124" s="145"/>
-      <c r="C124" s="145"/>
-      <c r="D124" s="145"/>
-      <c r="E124" s="145"/>
-      <c r="F124" s="145"/>
-      <c r="G124" s="145"/>
-      <c r="H124" s="145"/>
-      <c r="I124" s="145"/>
-      <c r="J124" s="145"/>
+      <c r="A124" s="146"/>
+      <c r="B124" s="146"/>
+      <c r="C124" s="146"/>
+      <c r="D124" s="146"/>
+      <c r="E124" s="146"/>
+      <c r="F124" s="146"/>
+      <c r="G124" s="146"/>
+      <c r="H124" s="146"/>
+      <c r="I124" s="146"/>
+      <c r="J124" s="146"/>
       <c r="K124" s="37"/>
       <c r="L124" s="69" t="s">
         <v>212</v>
@@ -28353,16 +28358,16 @@
       <c r="Z124" s="37"/>
     </row>
     <row r="125" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A125" s="145"/>
-      <c r="B125" s="145"/>
-      <c r="C125" s="145"/>
-      <c r="D125" s="145"/>
-      <c r="E125" s="145"/>
-      <c r="F125" s="145"/>
-      <c r="G125" s="145"/>
-      <c r="H125" s="145"/>
-      <c r="I125" s="145"/>
-      <c r="J125" s="145"/>
+      <c r="A125" s="146"/>
+      <c r="B125" s="146"/>
+      <c r="C125" s="146"/>
+      <c r="D125" s="146"/>
+      <c r="E125" s="146"/>
+      <c r="F125" s="146"/>
+      <c r="G125" s="146"/>
+      <c r="H125" s="146"/>
+      <c r="I125" s="146"/>
+      <c r="J125" s="146"/>
       <c r="K125" s="37"/>
       <c r="L125" s="67"/>
       <c r="M125" s="67"/>
@@ -28381,16 +28386,16 @@
       <c r="Z125" s="37"/>
     </row>
     <row r="126" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A126" s="145"/>
-      <c r="B126" s="145"/>
-      <c r="C126" s="145"/>
-      <c r="D126" s="145"/>
-      <c r="E126" s="145"/>
-      <c r="F126" s="145"/>
-      <c r="G126" s="145"/>
-      <c r="H126" s="145"/>
-      <c r="I126" s="145"/>
-      <c r="J126" s="145"/>
+      <c r="A126" s="146"/>
+      <c r="B126" s="146"/>
+      <c r="C126" s="146"/>
+      <c r="D126" s="146"/>
+      <c r="E126" s="146"/>
+      <c r="F126" s="146"/>
+      <c r="G126" s="146"/>
+      <c r="H126" s="146"/>
+      <c r="I126" s="146"/>
+      <c r="J126" s="146"/>
       <c r="K126" s="37"/>
       <c r="L126" s="67"/>
       <c r="M126" s="67"/>
@@ -28409,16 +28414,16 @@
       <c r="Z126" s="37"/>
     </row>
     <row r="127" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A127" s="145"/>
-      <c r="B127" s="145"/>
-      <c r="C127" s="145"/>
-      <c r="D127" s="145"/>
-      <c r="E127" s="145"/>
-      <c r="F127" s="145"/>
-      <c r="G127" s="145"/>
-      <c r="H127" s="145"/>
-      <c r="I127" s="145"/>
-      <c r="J127" s="145"/>
+      <c r="A127" s="146"/>
+      <c r="B127" s="146"/>
+      <c r="C127" s="146"/>
+      <c r="D127" s="146"/>
+      <c r="E127" s="146"/>
+      <c r="F127" s="146"/>
+      <c r="G127" s="146"/>
+      <c r="H127" s="146"/>
+      <c r="I127" s="146"/>
+      <c r="J127" s="146"/>
       <c r="K127" s="37"/>
       <c r="L127" s="67"/>
       <c r="M127" s="67"/>
@@ -28437,16 +28442,16 @@
       <c r="Z127" s="37"/>
     </row>
     <row r="128" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A128" s="145"/>
-      <c r="B128" s="145"/>
-      <c r="C128" s="145"/>
-      <c r="D128" s="145"/>
-      <c r="E128" s="145"/>
-      <c r="F128" s="145"/>
-      <c r="G128" s="145"/>
-      <c r="H128" s="145"/>
-      <c r="I128" s="145"/>
-      <c r="J128" s="145"/>
+      <c r="A128" s="146"/>
+      <c r="B128" s="146"/>
+      <c r="C128" s="146"/>
+      <c r="D128" s="146"/>
+      <c r="E128" s="146"/>
+      <c r="F128" s="146"/>
+      <c r="G128" s="146"/>
+      <c r="H128" s="146"/>
+      <c r="I128" s="146"/>
+      <c r="J128" s="146"/>
       <c r="K128" s="37"/>
       <c r="L128" s="67"/>
       <c r="M128" s="67"/>
@@ -28465,16 +28470,16 @@
       <c r="Z128" s="37"/>
     </row>
     <row r="129" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A129" s="145"/>
-      <c r="B129" s="145"/>
-      <c r="C129" s="145"/>
-      <c r="D129" s="145"/>
-      <c r="E129" s="145"/>
-      <c r="F129" s="145"/>
-      <c r="G129" s="145"/>
-      <c r="H129" s="145"/>
-      <c r="I129" s="145"/>
-      <c r="J129" s="145"/>
+      <c r="A129" s="146"/>
+      <c r="B129" s="146"/>
+      <c r="C129" s="146"/>
+      <c r="D129" s="146"/>
+      <c r="E129" s="146"/>
+      <c r="F129" s="146"/>
+      <c r="G129" s="146"/>
+      <c r="H129" s="146"/>
+      <c r="I129" s="146"/>
+      <c r="J129" s="146"/>
       <c r="K129" s="37"/>
       <c r="L129" s="67"/>
       <c r="M129" s="67"/>
@@ -28493,16 +28498,16 @@
       <c r="Z129" s="37"/>
     </row>
     <row r="130" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A130" s="145"/>
-      <c r="B130" s="145"/>
-      <c r="C130" s="145"/>
-      <c r="D130" s="145"/>
-      <c r="E130" s="145"/>
-      <c r="F130" s="145"/>
-      <c r="G130" s="145"/>
-      <c r="H130" s="145"/>
-      <c r="I130" s="145"/>
-      <c r="J130" s="145"/>
+      <c r="A130" s="146"/>
+      <c r="B130" s="146"/>
+      <c r="C130" s="146"/>
+      <c r="D130" s="146"/>
+      <c r="E130" s="146"/>
+      <c r="F130" s="146"/>
+      <c r="G130" s="146"/>
+      <c r="H130" s="146"/>
+      <c r="I130" s="146"/>
+      <c r="J130" s="146"/>
       <c r="K130" s="37"/>
       <c r="L130" s="67"/>
       <c r="M130" s="67"/>
@@ -28523,16 +28528,16 @@
       <c r="Z130" s="37"/>
     </row>
     <row r="131" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A131" s="145"/>
-      <c r="B131" s="145"/>
-      <c r="C131" s="145"/>
-      <c r="D131" s="145"/>
-      <c r="E131" s="145"/>
-      <c r="F131" s="145"/>
-      <c r="G131" s="145"/>
-      <c r="H131" s="145"/>
-      <c r="I131" s="145"/>
-      <c r="J131" s="145"/>
+      <c r="A131" s="146"/>
+      <c r="B131" s="146"/>
+      <c r="C131" s="146"/>
+      <c r="D131" s="146"/>
+      <c r="E131" s="146"/>
+      <c r="F131" s="146"/>
+      <c r="G131" s="146"/>
+      <c r="H131" s="146"/>
+      <c r="I131" s="146"/>
+      <c r="J131" s="146"/>
       <c r="K131" s="37"/>
       <c r="L131" s="67"/>
       <c r="M131" s="67"/>
@@ -28551,16 +28556,16 @@
       <c r="Z131" s="37"/>
     </row>
     <row r="132" spans="1:26" ht="30.75" customHeight="1">
-      <c r="A132" s="145"/>
-      <c r="B132" s="145"/>
-      <c r="C132" s="145"/>
-      <c r="D132" s="145"/>
-      <c r="E132" s="145"/>
-      <c r="F132" s="145"/>
-      <c r="G132" s="145"/>
-      <c r="H132" s="145"/>
-      <c r="I132" s="145"/>
-      <c r="J132" s="145"/>
+      <c r="A132" s="146"/>
+      <c r="B132" s="146"/>
+      <c r="C132" s="146"/>
+      <c r="D132" s="146"/>
+      <c r="E132" s="146"/>
+      <c r="F132" s="146"/>
+      <c r="G132" s="146"/>
+      <c r="H132" s="146"/>
+      <c r="I132" s="146"/>
+      <c r="J132" s="146"/>
       <c r="K132" s="37"/>
       <c r="L132" s="58"/>
       <c r="M132" s="58"/>
@@ -28579,16 +28584,16 @@
       <c r="Z132" s="37"/>
     </row>
     <row r="133" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A133" s="145"/>
-      <c r="B133" s="145"/>
-      <c r="C133" s="145"/>
-      <c r="D133" s="145"/>
-      <c r="E133" s="145"/>
-      <c r="F133" s="145"/>
-      <c r="G133" s="145"/>
-      <c r="H133" s="145"/>
-      <c r="I133" s="145"/>
-      <c r="J133" s="145"/>
+      <c r="A133" s="146"/>
+      <c r="B133" s="146"/>
+      <c r="C133" s="146"/>
+      <c r="D133" s="146"/>
+      <c r="E133" s="146"/>
+      <c r="F133" s="146"/>
+      <c r="G133" s="146"/>
+      <c r="H133" s="146"/>
+      <c r="I133" s="146"/>
+      <c r="J133" s="146"/>
       <c r="K133" s="37"/>
       <c r="L133" s="104"/>
       <c r="M133" s="106"/>
@@ -28607,16 +28612,16 @@
       <c r="Z133" s="37"/>
     </row>
     <row r="134" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A134" s="145"/>
-      <c r="B134" s="145"/>
-      <c r="C134" s="145"/>
-      <c r="D134" s="145"/>
-      <c r="E134" s="145"/>
-      <c r="F134" s="145"/>
-      <c r="G134" s="145"/>
-      <c r="H134" s="145"/>
-      <c r="I134" s="145"/>
-      <c r="J134" s="145"/>
+      <c r="A134" s="146"/>
+      <c r="B134" s="146"/>
+      <c r="C134" s="146"/>
+      <c r="D134" s="146"/>
+      <c r="E134" s="146"/>
+      <c r="F134" s="146"/>
+      <c r="G134" s="146"/>
+      <c r="H134" s="146"/>
+      <c r="I134" s="146"/>
+      <c r="J134" s="146"/>
       <c r="K134" s="37"/>
       <c r="L134" s="104"/>
       <c r="M134" s="106"/>
@@ -28635,16 +28640,16 @@
       <c r="Z134" s="37"/>
     </row>
     <row r="135" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A135" s="145"/>
-      <c r="B135" s="145"/>
-      <c r="C135" s="145"/>
-      <c r="D135" s="145"/>
-      <c r="E135" s="145"/>
-      <c r="F135" s="145"/>
-      <c r="G135" s="145"/>
-      <c r="H135" s="145"/>
-      <c r="I135" s="145"/>
-      <c r="J135" s="145"/>
+      <c r="A135" s="146"/>
+      <c r="B135" s="146"/>
+      <c r="C135" s="146"/>
+      <c r="D135" s="146"/>
+      <c r="E135" s="146"/>
+      <c r="F135" s="146"/>
+      <c r="G135" s="146"/>
+      <c r="H135" s="146"/>
+      <c r="I135" s="146"/>
+      <c r="J135" s="146"/>
       <c r="K135" s="37"/>
       <c r="L135" s="104"/>
       <c r="M135" s="106"/>
@@ -28663,16 +28668,16 @@
       <c r="Z135" s="37"/>
     </row>
     <row r="136" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A136" s="145"/>
-      <c r="B136" s="145"/>
-      <c r="C136" s="145"/>
-      <c r="D136" s="145"/>
-      <c r="E136" s="145"/>
-      <c r="F136" s="145"/>
-      <c r="G136" s="145"/>
-      <c r="H136" s="145"/>
-      <c r="I136" s="145"/>
-      <c r="J136" s="145"/>
+      <c r="A136" s="146"/>
+      <c r="B136" s="146"/>
+      <c r="C136" s="146"/>
+      <c r="D136" s="146"/>
+      <c r="E136" s="146"/>
+      <c r="F136" s="146"/>
+      <c r="G136" s="146"/>
+      <c r="H136" s="146"/>
+      <c r="I136" s="146"/>
+      <c r="J136" s="146"/>
       <c r="K136" s="37"/>
       <c r="L136" s="104"/>
       <c r="M136" s="106"/>
@@ -28691,16 +28696,16 @@
       <c r="Z136" s="37"/>
     </row>
     <row r="137" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A137" s="145"/>
-      <c r="B137" s="145"/>
-      <c r="C137" s="145"/>
-      <c r="D137" s="145"/>
-      <c r="E137" s="145"/>
-      <c r="F137" s="145"/>
-      <c r="G137" s="145"/>
-      <c r="H137" s="145"/>
-      <c r="I137" s="145"/>
-      <c r="J137" s="145"/>
+      <c r="A137" s="146"/>
+      <c r="B137" s="146"/>
+      <c r="C137" s="146"/>
+      <c r="D137" s="146"/>
+      <c r="E137" s="146"/>
+      <c r="F137" s="146"/>
+      <c r="G137" s="146"/>
+      <c r="H137" s="146"/>
+      <c r="I137" s="146"/>
+      <c r="J137" s="146"/>
       <c r="K137" s="37"/>
       <c r="L137" s="104"/>
       <c r="M137" s="106"/>
@@ -28719,16 +28724,16 @@
       <c r="Z137" s="37"/>
     </row>
     <row r="138" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A138" s="145"/>
-      <c r="B138" s="145"/>
-      <c r="C138" s="145"/>
-      <c r="D138" s="145"/>
-      <c r="E138" s="145"/>
-      <c r="F138" s="145"/>
-      <c r="G138" s="145"/>
-      <c r="H138" s="145"/>
-      <c r="I138" s="145"/>
-      <c r="J138" s="145"/>
+      <c r="A138" s="146"/>
+      <c r="B138" s="146"/>
+      <c r="C138" s="146"/>
+      <c r="D138" s="146"/>
+      <c r="E138" s="146"/>
+      <c r="F138" s="146"/>
+      <c r="G138" s="146"/>
+      <c r="H138" s="146"/>
+      <c r="I138" s="146"/>
+      <c r="J138" s="146"/>
       <c r="K138" s="37"/>
       <c r="L138" s="104"/>
       <c r="M138" s="106"/>
@@ -28747,16 +28752,16 @@
       <c r="Z138" s="37"/>
     </row>
     <row r="139" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A139" s="145"/>
-      <c r="B139" s="145"/>
-      <c r="C139" s="145"/>
-      <c r="D139" s="145"/>
-      <c r="E139" s="145"/>
-      <c r="F139" s="145"/>
-      <c r="G139" s="145"/>
-      <c r="H139" s="145"/>
-      <c r="I139" s="145"/>
-      <c r="J139" s="145"/>
+      <c r="A139" s="146"/>
+      <c r="B139" s="146"/>
+      <c r="C139" s="146"/>
+      <c r="D139" s="146"/>
+      <c r="E139" s="146"/>
+      <c r="F139" s="146"/>
+      <c r="G139" s="146"/>
+      <c r="H139" s="146"/>
+      <c r="I139" s="146"/>
+      <c r="J139" s="146"/>
       <c r="K139" s="37"/>
       <c r="L139" s="104"/>
       <c r="M139" s="106"/>
@@ -28775,16 +28780,16 @@
       <c r="Z139" s="37"/>
     </row>
     <row r="140" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A140" s="145"/>
-      <c r="B140" s="145"/>
-      <c r="C140" s="145"/>
-      <c r="D140" s="145"/>
-      <c r="E140" s="145"/>
-      <c r="F140" s="145"/>
-      <c r="G140" s="145"/>
-      <c r="H140" s="145"/>
-      <c r="I140" s="145"/>
-      <c r="J140" s="145"/>
+      <c r="A140" s="146"/>
+      <c r="B140" s="146"/>
+      <c r="C140" s="146"/>
+      <c r="D140" s="146"/>
+      <c r="E140" s="146"/>
+      <c r="F140" s="146"/>
+      <c r="G140" s="146"/>
+      <c r="H140" s="146"/>
+      <c r="I140" s="146"/>
+      <c r="J140" s="146"/>
       <c r="K140" s="37"/>
       <c r="L140" s="104"/>
       <c r="M140" s="106"/>
@@ -28803,16 +28808,16 @@
       <c r="Z140" s="37"/>
     </row>
     <row r="141" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A141" s="145"/>
-      <c r="B141" s="145"/>
-      <c r="C141" s="145"/>
-      <c r="D141" s="145"/>
-      <c r="E141" s="145"/>
-      <c r="F141" s="145"/>
-      <c r="G141" s="145"/>
-      <c r="H141" s="145"/>
-      <c r="I141" s="145"/>
-      <c r="J141" s="145"/>
+      <c r="A141" s="146"/>
+      <c r="B141" s="146"/>
+      <c r="C141" s="146"/>
+      <c r="D141" s="146"/>
+      <c r="E141" s="146"/>
+      <c r="F141" s="146"/>
+      <c r="G141" s="146"/>
+      <c r="H141" s="146"/>
+      <c r="I141" s="146"/>
+      <c r="J141" s="146"/>
       <c r="K141" s="37"/>
       <c r="L141" s="104"/>
       <c r="M141" s="106"/>
@@ -28831,16 +28836,16 @@
       <c r="Z141" s="37"/>
     </row>
     <row r="142" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A142" s="145"/>
-      <c r="B142" s="145"/>
-      <c r="C142" s="145"/>
-      <c r="D142" s="145"/>
-      <c r="E142" s="145"/>
-      <c r="F142" s="145"/>
-      <c r="G142" s="145"/>
-      <c r="H142" s="145"/>
-      <c r="I142" s="145"/>
-      <c r="J142" s="145"/>
+      <c r="A142" s="146"/>
+      <c r="B142" s="146"/>
+      <c r="C142" s="146"/>
+      <c r="D142" s="146"/>
+      <c r="E142" s="146"/>
+      <c r="F142" s="146"/>
+      <c r="G142" s="146"/>
+      <c r="H142" s="146"/>
+      <c r="I142" s="146"/>
+      <c r="J142" s="146"/>
       <c r="K142" s="37"/>
       <c r="L142" s="104"/>
       <c r="M142" s="106"/>
@@ -28859,16 +28864,16 @@
       <c r="Z142" s="37"/>
     </row>
     <row r="143" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A143" s="145"/>
-      <c r="B143" s="145"/>
-      <c r="C143" s="145"/>
-      <c r="D143" s="145"/>
-      <c r="E143" s="145"/>
-      <c r="F143" s="145"/>
-      <c r="G143" s="145"/>
-      <c r="H143" s="145"/>
-      <c r="I143" s="145"/>
-      <c r="J143" s="145"/>
+      <c r="A143" s="146"/>
+      <c r="B143" s="146"/>
+      <c r="C143" s="146"/>
+      <c r="D143" s="146"/>
+      <c r="E143" s="146"/>
+      <c r="F143" s="146"/>
+      <c r="G143" s="146"/>
+      <c r="H143" s="146"/>
+      <c r="I143" s="146"/>
+      <c r="J143" s="146"/>
       <c r="K143" s="37"/>
       <c r="L143" s="104"/>
       <c r="M143" s="106"/>
@@ -28887,16 +28892,16 @@
       <c r="Z143" s="37"/>
     </row>
     <row r="144" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A144" s="145"/>
-      <c r="B144" s="145"/>
-      <c r="C144" s="145"/>
-      <c r="D144" s="145"/>
-      <c r="E144" s="145"/>
-      <c r="F144" s="145"/>
-      <c r="G144" s="145"/>
-      <c r="H144" s="145"/>
-      <c r="I144" s="145"/>
-      <c r="J144" s="145"/>
+      <c r="A144" s="146"/>
+      <c r="B144" s="146"/>
+      <c r="C144" s="146"/>
+      <c r="D144" s="146"/>
+      <c r="E144" s="146"/>
+      <c r="F144" s="146"/>
+      <c r="G144" s="146"/>
+      <c r="H144" s="146"/>
+      <c r="I144" s="146"/>
+      <c r="J144" s="146"/>
       <c r="K144" s="37"/>
       <c r="L144" s="104"/>
       <c r="M144" s="106"/>
@@ -28915,16 +28920,16 @@
       <c r="Z144" s="37"/>
     </row>
     <row r="145" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A145" s="145"/>
-      <c r="B145" s="145"/>
-      <c r="C145" s="145"/>
-      <c r="D145" s="145"/>
-      <c r="E145" s="145"/>
-      <c r="F145" s="145"/>
-      <c r="G145" s="145"/>
-      <c r="H145" s="145"/>
-      <c r="I145" s="145"/>
-      <c r="J145" s="145"/>
+      <c r="A145" s="146"/>
+      <c r="B145" s="146"/>
+      <c r="C145" s="146"/>
+      <c r="D145" s="146"/>
+      <c r="E145" s="146"/>
+      <c r="F145" s="146"/>
+      <c r="G145" s="146"/>
+      <c r="H145" s="146"/>
+      <c r="I145" s="146"/>
+      <c r="J145" s="146"/>
       <c r="K145" s="37"/>
       <c r="L145" s="104"/>
       <c r="M145" s="106"/>
@@ -28943,16 +28948,16 @@
       <c r="Z145" s="37"/>
     </row>
     <row r="146" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A146" s="145"/>
-      <c r="B146" s="145"/>
-      <c r="C146" s="145"/>
-      <c r="D146" s="145"/>
-      <c r="E146" s="145"/>
-      <c r="F146" s="145"/>
-      <c r="G146" s="145"/>
-      <c r="H146" s="145"/>
-      <c r="I146" s="145"/>
-      <c r="J146" s="145"/>
+      <c r="A146" s="146"/>
+      <c r="B146" s="146"/>
+      <c r="C146" s="146"/>
+      <c r="D146" s="146"/>
+      <c r="E146" s="146"/>
+      <c r="F146" s="146"/>
+      <c r="G146" s="146"/>
+      <c r="H146" s="146"/>
+      <c r="I146" s="146"/>
+      <c r="J146" s="146"/>
       <c r="K146" s="37"/>
       <c r="L146" s="104"/>
       <c r="M146" s="106"/>
@@ -28971,16 +28976,16 @@
       <c r="Z146" s="37"/>
     </row>
     <row r="147" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A147" s="145"/>
-      <c r="B147" s="145"/>
-      <c r="C147" s="145"/>
-      <c r="D147" s="145"/>
-      <c r="E147" s="145"/>
-      <c r="F147" s="145"/>
-      <c r="G147" s="145"/>
-      <c r="H147" s="145"/>
-      <c r="I147" s="145"/>
-      <c r="J147" s="145"/>
+      <c r="A147" s="146"/>
+      <c r="B147" s="146"/>
+      <c r="C147" s="146"/>
+      <c r="D147" s="146"/>
+      <c r="E147" s="146"/>
+      <c r="F147" s="146"/>
+      <c r="G147" s="146"/>
+      <c r="H147" s="146"/>
+      <c r="I147" s="146"/>
+      <c r="J147" s="146"/>
       <c r="K147" s="37"/>
       <c r="L147" s="104"/>
       <c r="M147" s="106"/>
@@ -28999,16 +29004,16 @@
       <c r="Z147" s="37"/>
     </row>
     <row r="148" spans="1:26" ht="16.5" customHeight="1">
-      <c r="A148" s="145"/>
-      <c r="B148" s="145"/>
-      <c r="C148" s="145"/>
-      <c r="D148" s="145"/>
-      <c r="E148" s="145"/>
-      <c r="F148" s="145"/>
-      <c r="G148" s="145"/>
-      <c r="H148" s="145"/>
-      <c r="I148" s="145"/>
-      <c r="J148" s="145"/>
+      <c r="A148" s="146"/>
+      <c r="B148" s="146"/>
+      <c r="C148" s="146"/>
+      <c r="D148" s="146"/>
+      <c r="E148" s="146"/>
+      <c r="F148" s="146"/>
+      <c r="G148" s="146"/>
+      <c r="H148" s="146"/>
+      <c r="I148" s="146"/>
+      <c r="J148" s="146"/>
       <c r="K148" s="37"/>
       <c r="L148" s="104"/>
       <c r="M148" s="106"/>
@@ -29027,16 +29032,16 @@
       <c r="Z148" s="37"/>
     </row>
     <row r="149" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A149" s="145"/>
-      <c r="B149" s="145"/>
-      <c r="C149" s="145"/>
-      <c r="D149" s="145"/>
-      <c r="E149" s="145"/>
-      <c r="F149" s="145"/>
-      <c r="G149" s="145"/>
-      <c r="H149" s="145"/>
-      <c r="I149" s="145"/>
-      <c r="J149" s="145"/>
+      <c r="A149" s="146"/>
+      <c r="B149" s="146"/>
+      <c r="C149" s="146"/>
+      <c r="D149" s="146"/>
+      <c r="E149" s="146"/>
+      <c r="F149" s="146"/>
+      <c r="G149" s="146"/>
+      <c r="H149" s="146"/>
+      <c r="I149" s="146"/>
+      <c r="J149" s="146"/>
       <c r="K149" s="37"/>
       <c r="L149" s="104"/>
       <c r="M149" s="106"/>
@@ -31631,8 +31636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F55" sqref="F55"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -31780,7 +31785,7 @@
         <v>60</v>
       </c>
       <c r="C24" s="119" t="s">
-        <v>70</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="2:3">
@@ -34856,8 +34861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="G67" sqref="G67"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H49" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -35325,73 +35330,84 @@
       </c>
       <c r="L42" s="131"/>
     </row>
+    <row r="43" spans="2:12" ht="15" customHeight="1">
+      <c r="B43" s="138" t="s">
+        <v>337</v>
+      </c>
+      <c r="C43" s="140"/>
+      <c r="D43" s="140"/>
+      <c r="E43" s="140"/>
+      <c r="F43" s="141"/>
+    </row>
     <row r="44" spans="2:12" ht="15" customHeight="1">
-      <c r="B44" s="138" t="s">
-        <v>337</v>
-      </c>
-      <c r="C44" s="140"/>
-      <c r="D44" s="140"/>
-      <c r="E44" s="140"/>
-      <c r="F44" s="141"/>
+      <c r="B44" s="137" t="s">
+        <v>298</v>
+      </c>
+      <c r="C44" s="133"/>
+      <c r="D44" s="133"/>
+      <c r="E44" s="133" t="s">
+        <v>301</v>
+      </c>
+      <c r="F44" s="134" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="45" spans="2:12" ht="15" customHeight="1">
       <c r="B45" s="137" t="s">
-        <v>298</v>
+        <v>241</v>
       </c>
       <c r="C45" s="133"/>
       <c r="D45" s="133"/>
       <c r="E45" s="133" t="s">
-        <v>301</v>
-      </c>
-      <c r="F45" s="134" t="s">
-        <v>303</v>
-      </c>
+        <v>302</v>
+      </c>
+      <c r="F45" s="134"/>
     </row>
     <row r="46" spans="2:12" ht="15" customHeight="1">
       <c r="B46" s="137" t="s">
-        <v>241</v>
+        <v>338</v>
       </c>
       <c r="C46" s="133"/>
       <c r="D46" s="133"/>
       <c r="E46" s="133" t="s">
-        <v>302</v>
-      </c>
-      <c r="F46" s="134"/>
+        <v>301</v>
+      </c>
+      <c r="F46" s="134" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="47" spans="2:12" ht="15" customHeight="1">
       <c r="B47" s="137" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="C47" s="133"/>
       <c r="D47" s="133"/>
       <c r="E47" s="133" t="s">
         <v>301</v>
       </c>
-      <c r="F47" s="134" t="s">
-        <v>304</v>
-      </c>
+      <c r="F47" s="134"/>
     </row>
     <row r="48" spans="2:12" ht="15" customHeight="1">
       <c r="B48" s="137" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="C48" s="133"/>
       <c r="D48" s="133"/>
       <c r="E48" s="133" t="s">
+        <v>302</v>
+      </c>
+      <c r="F48" s="134"/>
+    </row>
+    <row r="49" spans="2:12" ht="15" customHeight="1">
+      <c r="B49" s="135" t="s">
+        <v>367</v>
+      </c>
+      <c r="C49" s="130"/>
+      <c r="D49" s="130"/>
+      <c r="E49" s="144" t="s">
         <v>301</v>
       </c>
-      <c r="F48" s="134"/>
-    </row>
-    <row r="49" spans="2:12" ht="15" customHeight="1">
-      <c r="B49" s="139" t="s">
-        <v>340</v>
-      </c>
-      <c r="C49" s="136"/>
-      <c r="D49" s="136"/>
-      <c r="E49" s="136" t="s">
-        <v>302</v>
-      </c>
-      <c r="F49" s="142"/>
+      <c r="F49" s="131"/>
     </row>
     <row r="51" spans="2:12" ht="15" customHeight="1">
       <c r="B51" s="138" t="s">
@@ -35529,7 +35545,7 @@
       </c>
       <c r="C63" s="127"/>
       <c r="D63" s="127"/>
-      <c r="E63" s="149" t="s">
+      <c r="E63" s="143" t="s">
         <v>302</v>
       </c>
       <c r="F63" s="128"/>
@@ -35540,7 +35556,7 @@
       </c>
       <c r="C64" s="127"/>
       <c r="D64" s="127"/>
-      <c r="E64" s="149" t="s">
+      <c r="E64" s="143" t="s">
         <v>302</v>
       </c>
       <c r="F64" s="128"/>
@@ -35554,7 +35570,7 @@
       </c>
       <c r="C65" s="130"/>
       <c r="D65" s="130"/>
-      <c r="E65" s="150" t="s">
+      <c r="E65" s="144" t="s">
         <v>302</v>
       </c>
       <c r="F65" s="131"/>
@@ -35577,7 +35593,7 @@
       </c>
       <c r="C68" s="127"/>
       <c r="D68" s="127"/>
-      <c r="E68" s="143" t="s">
+      <c r="E68" s="142" t="s">
         <v>301</v>
       </c>
       <c r="F68" s="128"/>
@@ -35588,7 +35604,7 @@
       </c>
       <c r="C69" s="127"/>
       <c r="D69" s="127"/>
-      <c r="E69" s="143" t="s">
+      <c r="E69" s="142" t="s">
         <v>302</v>
       </c>
       <c r="F69" s="128"/>
@@ -35599,7 +35615,7 @@
       </c>
       <c r="C70" s="127"/>
       <c r="D70" s="127"/>
-      <c r="E70" s="143" t="s">
+      <c r="E70" s="142" t="s">
         <v>301</v>
       </c>
       <c r="F70" s="128"/>
@@ -35623,8 +35639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="15.140625" defaultRowHeight="15" customHeight="1"/>
@@ -35757,7 +35773,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:6">
       <c r="B17" s="119" t="s">
         <v>357</v>
       </c>
@@ -35765,7 +35781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:6">
       <c r="B18" s="119" t="s">
         <v>361</v>
       </c>
@@ -35773,7 +35789,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:6">
       <c r="B19" s="119" t="s">
         <v>358</v>
       </c>
@@ -35781,15 +35797,18 @@
         <v>359</v>
       </c>
     </row>
-    <row r="20" spans="2:4">
+    <row r="20" spans="2:6">
       <c r="B20" s="119" t="s">
         <v>360</v>
       </c>
       <c r="D20" s="123" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="21" spans="2:4">
+      <c r="F20" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6">
       <c r="B21" s="119" t="s">
         <v>362</v>
       </c>
@@ -35797,37 +35816,37 @@
         <v>274</v>
       </c>
     </row>
-    <row r="22" spans="2:4">
+    <row r="22" spans="2:6">
       <c r="B22" s="1"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:6">
       <c r="B23" s="1"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:6">
       <c r="B24" s="1"/>
     </row>
-    <row r="25" spans="2:4">
+    <row r="25" spans="2:6">
       <c r="B25" s="1"/>
     </row>
-    <row r="26" spans="2:4">
+    <row r="26" spans="2:6">
       <c r="B26" s="1"/>
     </row>
-    <row r="27" spans="2:4">
+    <row r="27" spans="2:6">
       <c r="B27" s="1"/>
     </row>
-    <row r="28" spans="2:4">
+    <row r="28" spans="2:6">
       <c r="B28" s="1"/>
     </row>
-    <row r="29" spans="2:4">
+    <row r="29" spans="2:6">
       <c r="B29" s="1"/>
     </row>
-    <row r="30" spans="2:4">
+    <row r="30" spans="2:6">
       <c r="B30" s="1"/>
     </row>
-    <row r="31" spans="2:4">
+    <row r="31" spans="2:6">
       <c r="B31" s="1"/>
     </row>
-    <row r="32" spans="2:4">
+    <row r="32" spans="2:6">
       <c r="B32" s="1"/>
     </row>
     <row r="33" spans="2:2">

</xml_diff>